<commit_message>
Evaluation Protocol once again
</commit_message>
<xml_diff>
--- a/JS SPA Self Evaluation Protocol.xlsx
+++ b/JS SPA Self Evaluation Protocol.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="60">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -190,13 +190,22 @@
   </si>
   <si>
     <t>∞</t>
+  </si>
+  <si>
+    <t>rafatpc</t>
+  </si>
+  <si>
+    <t>Liliyan Krumov</t>
+  </si>
+  <si>
+    <t>https://github.com/rafatpc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,6 +235,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -321,10 +338,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -376,8 +394,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -648,7 +670,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -658,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:E10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,7 +717,9 @@
       <c r="B4" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="17"/>
+      <c r="C4" s="17" t="s">
+        <v>57</v>
+      </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
     </row>
@@ -703,7 +727,9 @@
       <c r="B5" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="17"/>
+      <c r="C5" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
     </row>
@@ -719,7 +745,9 @@
       <c r="B7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="20"/>
+      <c r="C7" s="21" t="s">
+        <v>59</v>
+      </c>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
     </row>
@@ -1220,7 +1248,10 @@
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="C7:E7"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C7" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Evaluation Protocol once again x2
</commit_message>
<xml_diff>
--- a/JS SPA Self Evaluation Protocol.xlsx
+++ b/JS SPA Self Evaluation Protocol.xlsx
@@ -391,10 +391,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -670,7 +670,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -680,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:E5"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,11 +745,11 @@
       <c r="B7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
@@ -768,7 +768,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="6">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>56</v>
@@ -800,7 +800,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>5</v>
@@ -860,7 +860,7 @@
         <v>7</v>
       </c>
       <c r="C17" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>3</v>
@@ -1040,7 +1040,7 @@
         <v>24</v>
       </c>
       <c r="C32" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>5</v>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>